<commit_message>
modification des taches dans le diagrammes de pert
</commit_message>
<xml_diff>
--- a/Taches_modified.xlsx
+++ b/Taches_modified.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <t>_</t>
   </si>
   <si>
-    <t>E,F,I</t>
+    <t>C,F,H</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +693,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
@@ -712,14 +712,14 @@
         <v>44681</v>
       </c>
       <c r="D11" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>44693</v>
+        <v>44691</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -731,17 +731,17 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>44693</v>
+        <v>44691</v>
       </c>
       <c r="D12" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>44698</v>
+        <v>44695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>